<commit_message>
Prueba para el 4º año
</commit_message>
<xml_diff>
--- a/comprobaciones.xlsx
+++ b/comprobaciones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josemorannebot/Desktop/CEU/TFG/TFG_Jose_Moran/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F62F7499-279B-AA45-BB20-7600CE1D0FDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3190DF1-1A0A-BE4F-8ABE-1998CD39C136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{C8D28FA2-159E-9546-8F5E-B1E8C848320B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14320" xr2:uid="{C8D28FA2-159E-9546-8F5E-B1E8C848320B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="187">
   <si>
     <t>order(1,0,0)</t>
   </si>
@@ -558,6 +558,45 @@
   </si>
   <si>
     <t>Prob(H) (two-sided):                  0.36   Kurtosis:                         4.06</t>
+  </si>
+  <si>
+    <t>order(0,2,2)</t>
+  </si>
+  <si>
+    <t>Model:             ARIMA(0, 2, 2)x(1, 0, [], 52)   Log Likelihood                -439.473</t>
+  </si>
+  <si>
+    <t>Date:                           Thu, 04 May 2023   AIC                            886.945</t>
+  </si>
+  <si>
+    <t>Time:                                   19:38:26   BIC                            897.445</t>
+  </si>
+  <si>
+    <t>Sample:                               01-06-2013   HQIC                           891.197</t>
+  </si>
+  <si>
+    <t>ma.L1         -1.3222      0.112    -11.762      0.000      -1.543      -1.102</t>
+  </si>
+  <si>
+    <t>ma.L2          0.3788      0.112      3.394      0.001       0.160       0.598</t>
+  </si>
+  <si>
+    <t>ar.S.L52       0.4127      0.156      2.646      0.008       0.107       0.718</t>
+  </si>
+  <si>
+    <t>sigma2       286.2706     50.515      5.667      0.000     187.262     385.279</t>
+  </si>
+  <si>
+    <t>Ljung-Box (L1) (Q):                   0.30   Jarque-Bera (JB):                 9.19</t>
+  </si>
+  <si>
+    <t>Prob(Q):                              0.58   Prob(JB):                         0.01</t>
+  </si>
+  <si>
+    <t>Heteroskedasticity (H):               0.93   Skew:                             0.61</t>
+  </si>
+  <si>
+    <t>Prob(H) (two-sided):                  0.83   Kurtosis:                         3.82</t>
   </si>
 </sst>
 </file>
@@ -565,7 +604,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="#,##0.000000000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.000000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -630,7 +669,7 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -947,10 +986,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A92E8C9-35F4-B741-A819-D77163E4CC90}">
-  <dimension ref="A1:P165"/>
+  <dimension ref="A1:Q169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
-      <selection activeCell="E165" sqref="E165"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73:B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1101,7 +1140,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
         <v>18</v>
       </c>
@@ -1109,7 +1148,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
         <v>19</v>
       </c>
@@ -1117,7 +1156,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
         <v>20</v>
       </c>
@@ -1125,7 +1164,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
         <v>21</v>
       </c>
@@ -1133,7 +1172,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
         <v>22</v>
       </c>
@@ -1141,7 +1180,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
         <v>18</v>
       </c>
@@ -1151,16 +1190,22 @@
       <c r="P22" s="1">
         <v>248.19711762184301</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
         <v>23</v>
       </c>
       <c r="D23" s="2">
         <v>392.57372687998401</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="E23">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="L24" s="1" t="s">
         <v>87</v>
       </c>
@@ -1171,7 +1216,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
@@ -1185,7 +1230,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
         <v>3</v>
       </c>
@@ -1193,7 +1238,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
         <v>4</v>
       </c>
@@ -1201,7 +1246,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C28" t="s">
         <v>26</v>
       </c>
@@ -1209,7 +1254,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
         <v>27</v>
       </c>
@@ -1217,7 +1262,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
         <v>28</v>
       </c>
@@ -1225,7 +1270,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
         <v>29</v>
       </c>
@@ -1233,7 +1278,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C32" t="s">
         <v>9</v>
       </c>
@@ -1241,7 +1286,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C33" t="s">
         <v>10</v>
       </c>
@@ -1249,7 +1294,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C34" t="s">
         <v>11</v>
       </c>
@@ -1257,7 +1302,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C35" t="s">
         <v>12</v>
       </c>
@@ -1265,7 +1310,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C36" t="s">
         <v>13</v>
       </c>
@@ -1273,7 +1318,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C37" t="s">
         <v>30</v>
       </c>
@@ -1281,7 +1326,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C38" t="s">
         <v>31</v>
       </c>
@@ -1289,7 +1334,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C39" t="s">
         <v>32</v>
       </c>
@@ -1297,7 +1342,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C40" t="s">
         <v>18</v>
       </c>
@@ -1305,7 +1350,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C41" t="s">
         <v>33</v>
       </c>
@@ -1313,7 +1358,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C42" t="s">
         <v>34</v>
       </c>
@@ -1321,7 +1366,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C43" t="s">
         <v>35</v>
       </c>
@@ -1329,7 +1374,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C44" t="s">
         <v>36</v>
       </c>
@@ -1337,7 +1382,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C45" t="s">
         <v>18</v>
       </c>
@@ -1345,26 +1390,32 @@
         <v>104</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C46" t="s">
         <v>23</v>
       </c>
       <c r="D46" s="1">
         <v>516.20296382784397</v>
       </c>
+      <c r="E46">
+        <v>13</v>
+      </c>
       <c r="O46" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="O47" t="s">
         <v>23</v>
       </c>
       <c r="P47" s="1">
         <v>461.87241507368901</v>
       </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q47">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>0</v>
       </c>
@@ -1509,7 +1560,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C65" t="s">
         <v>18</v>
       </c>
@@ -1517,7 +1568,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C66" t="s">
         <v>52</v>
       </c>
@@ -1525,7 +1576,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C67" t="s">
         <v>20</v>
       </c>
@@ -1533,7 +1584,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C68" t="s">
         <v>53</v>
       </c>
@@ -1541,7 +1592,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C69" t="s">
         <v>54</v>
       </c>
@@ -1549,7 +1600,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C70" t="s">
         <v>18</v>
       </c>
@@ -1557,21 +1608,27 @@
         <v>18</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C71" t="s">
         <v>23</v>
       </c>
       <c r="D71" s="1">
         <v>495.33237782125502</v>
       </c>
+      <c r="E71">
+        <v>10</v>
+      </c>
       <c r="O71" t="s">
         <v>23</v>
       </c>
       <c r="P71" s="1">
         <v>501.92337258799603</v>
       </c>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q71">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>0</v>
       </c>
@@ -1591,7 +1648,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C74" t="s">
         <v>39</v>
       </c>
@@ -1599,7 +1656,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C75" t="s">
         <v>40</v>
       </c>
@@ -1607,7 +1664,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C76" t="s">
         <v>56</v>
       </c>
@@ -1615,7 +1672,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C77" t="s">
         <v>57</v>
       </c>
@@ -1623,7 +1680,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C78" t="s">
         <v>58</v>
       </c>
@@ -1631,7 +1688,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C79" t="s">
         <v>59</v>
       </c>
@@ -1639,7 +1696,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C80" t="s">
         <v>45</v>
       </c>
@@ -1647,7 +1704,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="81" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C81" t="s">
         <v>46</v>
       </c>
@@ -1655,7 +1712,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="82" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C82" t="s">
         <v>11</v>
       </c>
@@ -1663,7 +1720,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="83" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="83" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C83" t="s">
         <v>12</v>
       </c>
@@ -1671,7 +1728,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="84" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C84" t="s">
         <v>13</v>
       </c>
@@ -1679,7 +1736,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="85" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="85" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C85" t="s">
         <v>60</v>
       </c>
@@ -1687,7 +1744,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="86" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="86" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C86" t="s">
         <v>61</v>
       </c>
@@ -1695,7 +1752,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="87" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="87" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C87" t="s">
         <v>62</v>
       </c>
@@ -1703,7 +1760,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="88" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="88" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C88" t="s">
         <v>63</v>
       </c>
@@ -1711,7 +1768,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="89" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="89" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C89" t="s">
         <v>18</v>
       </c>
@@ -1719,7 +1776,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="90" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="90" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C90" t="s">
         <v>33</v>
       </c>
@@ -1727,7 +1784,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="91" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="91" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C91" t="s">
         <v>34</v>
       </c>
@@ -1735,7 +1792,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="92" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="92" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C92" t="s">
         <v>35</v>
       </c>
@@ -1743,7 +1800,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="93" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="93" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C93" t="s">
         <v>36</v>
       </c>
@@ -1751,7 +1808,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="94" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="94" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C94" t="s">
         <v>18</v>
       </c>
@@ -1759,23 +1816,29 @@
         <v>116</v>
       </c>
     </row>
-    <row r="95" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="95" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C95" t="s">
         <v>23</v>
       </c>
       <c r="D95" s="1">
         <v>534.74548954856095</v>
       </c>
+      <c r="E95">
+        <v>14</v>
+      </c>
       <c r="O95" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="96" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="96" spans="3:17" x14ac:dyDescent="0.2">
       <c r="O96" t="s">
         <v>23</v>
       </c>
       <c r="P96" s="1">
         <v>504.69233627817698</v>
+      </c>
+      <c r="Q96">
+        <v>12</v>
       </c>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.2">
@@ -1915,7 +1978,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C113" t="s">
         <v>72</v>
       </c>
@@ -1923,7 +1986,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C114" t="s">
         <v>73</v>
       </c>
@@ -1931,7 +1994,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C115" t="s">
         <v>74</v>
       </c>
@@ -1939,7 +2002,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C116" t="s">
         <v>18</v>
       </c>
@@ -1947,23 +2010,26 @@
         <v>136</v>
       </c>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C117" t="s">
         <v>23</v>
       </c>
       <c r="D117" s="1">
         <v>466.55711809575303</v>
       </c>
+      <c r="E117">
+        <v>9</v>
+      </c>
       <c r="O117" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.2">
       <c r="O118" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>152</v>
       </c>
@@ -1977,7 +2043,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C120" t="s">
         <v>88</v>
       </c>
@@ -1987,13 +2053,16 @@
       <c r="P120" s="1">
         <v>248.64241124203301</v>
       </c>
-    </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q120">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="121" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C121" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C122" t="s">
         <v>153</v>
       </c>
@@ -2007,7 +2076,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C123" t="s">
         <v>154</v>
       </c>
@@ -2015,7 +2084,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C124" t="s">
         <v>155</v>
       </c>
@@ -2023,7 +2092,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C125" t="s">
         <v>156</v>
       </c>
@@ -2031,7 +2100,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C126" t="s">
         <v>94</v>
       </c>
@@ -2039,7 +2108,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C127" t="s">
         <v>95</v>
       </c>
@@ -2047,7 +2116,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C128" t="s">
         <v>11</v>
       </c>
@@ -2158,6 +2227,9 @@
       <c r="D141" s="1">
         <v>248.540270626758</v>
       </c>
+      <c r="E141">
+        <v>5</v>
+      </c>
       <c r="O141" t="s">
         <v>149</v>
       </c>
@@ -2189,7 +2261,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="145" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="145" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C145" t="s">
         <v>3</v>
       </c>
@@ -2199,108 +2271,203 @@
       <c r="P145" s="1">
         <v>248.440281304563</v>
       </c>
-    </row>
-    <row r="146" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="Q145">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="146" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C146" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="147" spans="3:16" x14ac:dyDescent="0.2">
+    <row r="147" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C147" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="148" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="L147" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="M147" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O147" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="148" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C148" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="149" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="O148" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="149" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C149" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="150" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="O149" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="150" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C150" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="151" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="O150" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="151" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C151" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="152" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="O151" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="152" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C152" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="153" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="O152" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="153" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C153" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="154" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="O153" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="154" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C154" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="155" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="O154" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="155" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C155" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="156" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="O155" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="156" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C156" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="157" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="O156" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="157" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C157" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="158" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="O157" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="158" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C158" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="159" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="O158" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="159" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C159" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="160" spans="3:16" x14ac:dyDescent="0.2">
+      <c r="O159" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="160" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C160" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="161" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="O160" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="161" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C161" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="162" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="O161" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="162" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C162" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="163" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="O162" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="163" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C163" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="164" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="O163" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="164" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C164" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="165" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="O164" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="165" spans="3:17" x14ac:dyDescent="0.2">
       <c r="C165" t="s">
         <v>23</v>
       </c>
       <c r="D165" s="1">
         <v>236.28383130894301</v>
+      </c>
+      <c r="E165">
+        <v>2</v>
+      </c>
+      <c r="O165" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="166" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="O166" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="167" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="O167" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="168" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="O168" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="169" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="O169" t="s">
+        <v>23</v>
+      </c>
+      <c r="P169" s="1">
+        <v>203.87327444989899</v>
+      </c>
+      <c r="Q169">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>